<commit_message>
Final cleaning for submission 01/09
</commit_message>
<xml_diff>
--- a/data/Carbon_Footprint_Secondary.xlsx
+++ b/data/Carbon_Footprint_Secondary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB6F3E0-665C-47EE-9C9D-FC0BA0CE8D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696BF313-5ECF-4DC7-B6E4-1F98184D17AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{14E8540C-EDEE-4050-9B8C-8C7F8EC6EA2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{14E8540C-EDEE-4050-9B8C-8C7F8EC6EA2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -6216,7 +6216,7 @@
       <sheetName val="Data_prep"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="102">
           <cell r="A102">
@@ -6933,7 +6933,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7736,7 +7736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B104145-72CF-4536-9B2E-C849D28231C3}">
   <dimension ref="A1:D152"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -10331,7 +10331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD439C0-9D31-45BF-BF24-D7490C893411}">
   <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G164" sqref="G164"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed secondary carbon footprint
In the data file Carbon_Footprint_Secondary.xlsx, the name of the Constant scenario for carbon footprint was wrong, leading to carbon footprint for secondary production not being accounted for
</commit_message>
<xml_diff>
--- a/data/Carbon_Footprint_Secondary.xlsx
+++ b/data/Carbon_Footprint_Secondary.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696BF313-5ECF-4DC7-B6E4-1F98184D17AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E3693-4C3A-4612-9DA0-80F86AAFB40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{14E8540C-EDEE-4050-9B8C-8C7F8EC6EA2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{14E8540C-EDEE-4050-9B8C-8C7F8EC6EA2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="4" r:id="rId2"/>
     <sheet name="Data_prep" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -453,7 +450,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BAU</c:v>
+                  <c:v>Constant</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6207,738 +6204,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Data"/>
-      <sheetName val="Data_prep"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="102">
-          <cell r="A102">
-            <v>2000</v>
-          </cell>
-          <cell r="B102">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="C102">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="D102">
-            <v>17.71089224218062</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103">
-            <v>2001</v>
-          </cell>
-          <cell r="B103">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="C103">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="D103">
-            <v>17.71089224218062</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="A104">
-            <v>2002</v>
-          </cell>
-          <cell r="B104">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="C104">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="D104">
-            <v>17.71089224218062</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="A105">
-            <v>2003</v>
-          </cell>
-          <cell r="B105">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="C105">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="D105">
-            <v>17.71089224218062</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="A106">
-            <v>2004</v>
-          </cell>
-          <cell r="B106">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="C106">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="D106">
-            <v>17.71089224218062</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="A107">
-            <v>2005</v>
-          </cell>
-          <cell r="B107">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="C107">
-            <v>17.71089224218062</v>
-          </cell>
-          <cell r="D107">
-            <v>17.71089224218062</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="A108">
-            <v>2006</v>
-          </cell>
-          <cell r="B108">
-            <v>18.505836116044783</v>
-          </cell>
-          <cell r="C108">
-            <v>18.505836116044783</v>
-          </cell>
-          <cell r="D108">
-            <v>18.505836116044783</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="A109">
-            <v>2007</v>
-          </cell>
-          <cell r="B109">
-            <v>18.842946447321911</v>
-          </cell>
-          <cell r="C109">
-            <v>18.842946447321911</v>
-          </cell>
-          <cell r="D109">
-            <v>18.842946447321911</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="A110">
-            <v>2008</v>
-          </cell>
-          <cell r="B110">
-            <v>18.456260621912495</v>
-          </cell>
-          <cell r="C110">
-            <v>18.456260621912495</v>
-          </cell>
-          <cell r="D110">
-            <v>18.456260621912495</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="A111">
-            <v>2009</v>
-          </cell>
-          <cell r="B111">
-            <v>18.106913183078134</v>
-          </cell>
-          <cell r="C111">
-            <v>18.106913183078134</v>
-          </cell>
-          <cell r="D111">
-            <v>18.106913183078134</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="A112">
-            <v>2010</v>
-          </cell>
-          <cell r="B112">
-            <v>17.463165009112874</v>
-          </cell>
-          <cell r="C112">
-            <v>17.463165009112874</v>
-          </cell>
-          <cell r="D112">
-            <v>17.463165009112874</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="A113">
-            <v>2011</v>
-          </cell>
-          <cell r="B113">
-            <v>17.688074803973674</v>
-          </cell>
-          <cell r="C113">
-            <v>17.688074803973674</v>
-          </cell>
-          <cell r="D113">
-            <v>17.688074803973674</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="A114">
-            <v>2012</v>
-          </cell>
-          <cell r="B114">
-            <v>18.174037618731763</v>
-          </cell>
-          <cell r="C114">
-            <v>18.174037618731763</v>
-          </cell>
-          <cell r="D114">
-            <v>18.174037618731763</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="A115">
-            <v>2013</v>
-          </cell>
-          <cell r="B115">
-            <v>18.041895342779902</v>
-          </cell>
-          <cell r="C115">
-            <v>18.041895342779902</v>
-          </cell>
-          <cell r="D115">
-            <v>18.041895342779902</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="A116">
-            <v>2014</v>
-          </cell>
-          <cell r="B116">
-            <v>18.067924587946695</v>
-          </cell>
-          <cell r="C116">
-            <v>18.067924587946695</v>
-          </cell>
-          <cell r="D116">
-            <v>18.067924587946695</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="A117">
-            <v>2015</v>
-          </cell>
-          <cell r="B117">
-            <v>16.970000000000002</v>
-          </cell>
-          <cell r="C117">
-            <v>16.970000000000002</v>
-          </cell>
-          <cell r="D117">
-            <v>16.970000000000002</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="A118">
-            <v>2016</v>
-          </cell>
-          <cell r="B118">
-            <v>16.885359650208649</v>
-          </cell>
-          <cell r="C118">
-            <v>16.885359650208649</v>
-          </cell>
-          <cell r="D118">
-            <v>16.885359650208649</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="A119">
-            <v>2017</v>
-          </cell>
-          <cell r="B119">
-            <v>16.892102171097623</v>
-          </cell>
-          <cell r="C119">
-            <v>16.892102171097623</v>
-          </cell>
-          <cell r="D119">
-            <v>16.892102171097623</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="A120">
-            <v>2018</v>
-          </cell>
-          <cell r="B120">
-            <v>16.912131261756848</v>
-          </cell>
-          <cell r="C120">
-            <v>16.912131261756848</v>
-          </cell>
-          <cell r="D120">
-            <v>16.912131261756848</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="A121">
-            <v>2019</v>
-          </cell>
-          <cell r="B121">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C121">
-            <v>16.807862195425926</v>
-          </cell>
-          <cell r="D121">
-            <v>16.807862195425926</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="A122">
-            <v>2020</v>
-          </cell>
-          <cell r="B122">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C122">
-            <v>16.643511086750841</v>
-          </cell>
-          <cell r="D122">
-            <v>16.66567017765993</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="A123">
-            <v>2021</v>
-          </cell>
-          <cell r="B123">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C123">
-            <v>16.479159978075756</v>
-          </cell>
-          <cell r="D123">
-            <v>16.523478159893937</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="A124">
-            <v>2022</v>
-          </cell>
-          <cell r="B124">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C124">
-            <v>16.314808869400672</v>
-          </cell>
-          <cell r="D124">
-            <v>16.381286142127944</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="A125">
-            <v>2023</v>
-          </cell>
-          <cell r="B125">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C125">
-            <v>16.150457760725587</v>
-          </cell>
-          <cell r="D125">
-            <v>16.239094124361952</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="A126">
-            <v>2024</v>
-          </cell>
-          <cell r="B126">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C126">
-            <v>15.986106652050502</v>
-          </cell>
-          <cell r="D126">
-            <v>16.096902106595959</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="A127">
-            <v>2025</v>
-          </cell>
-          <cell r="B127">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C127">
-            <v>15.821755543375417</v>
-          </cell>
-          <cell r="D127">
-            <v>15.954710088829964</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="A128">
-            <v>2026</v>
-          </cell>
-          <cell r="B128">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C128">
-            <v>15.657404434700332</v>
-          </cell>
-          <cell r="D128">
-            <v>15.81251807106397</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="A129">
-            <v>2027</v>
-          </cell>
-          <cell r="B129">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C129">
-            <v>15.493053326025247</v>
-          </cell>
-          <cell r="D129">
-            <v>15.670326053297977</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="A130">
-            <v>2028</v>
-          </cell>
-          <cell r="B130">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C130">
-            <v>15.328702217350163</v>
-          </cell>
-          <cell r="D130">
-            <v>15.528134035531984</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="A131">
-            <v>2029</v>
-          </cell>
-          <cell r="B131">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C131">
-            <v>15.164351108675078</v>
-          </cell>
-          <cell r="D131">
-            <v>15.38594201776599</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="A132">
-            <v>2030</v>
-          </cell>
-          <cell r="B132">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C132">
-            <v>15</v>
-          </cell>
-          <cell r="D132">
-            <v>15.24375</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="A133">
-            <v>2031</v>
-          </cell>
-          <cell r="B133">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C133">
-            <v>14.75</v>
-          </cell>
-          <cell r="D133">
-            <v>14.614062499999999</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="A134">
-            <v>2032</v>
-          </cell>
-          <cell r="B134">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C134">
-            <v>14.5</v>
-          </cell>
-          <cell r="D134">
-            <v>13.984375</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="A135">
-            <v>2033</v>
-          </cell>
-          <cell r="B135">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C135">
-            <v>14.25</v>
-          </cell>
-          <cell r="D135">
-            <v>13.354687500000001</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="A136">
-            <v>2034</v>
-          </cell>
-          <cell r="B136">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C136">
-            <v>14</v>
-          </cell>
-          <cell r="D136">
-            <v>12.725</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="A137">
-            <v>2035</v>
-          </cell>
-          <cell r="B137">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C137">
-            <v>13.75</v>
-          </cell>
-          <cell r="D137">
-            <v>12.0953125</v>
-          </cell>
-        </row>
-        <row r="138">
-          <cell r="A138">
-            <v>2036</v>
-          </cell>
-          <cell r="B138">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C138">
-            <v>13.5</v>
-          </cell>
-          <cell r="D138">
-            <v>11.465624999999999</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="A139">
-            <v>2037</v>
-          </cell>
-          <cell r="B139">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C139">
-            <v>13.25</v>
-          </cell>
-          <cell r="D139">
-            <v>10.8359375</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="A140">
-            <v>2038</v>
-          </cell>
-          <cell r="B140">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C140">
-            <v>13</v>
-          </cell>
-          <cell r="D140">
-            <v>10.206249999999999</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="A141">
-            <v>2039</v>
-          </cell>
-          <cell r="B141">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C141">
-            <v>12.75</v>
-          </cell>
-          <cell r="D141">
-            <v>9.5765624999999996</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="A142">
-            <v>2040</v>
-          </cell>
-          <cell r="B142">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C142">
-            <v>12.5</v>
-          </cell>
-          <cell r="D142">
-            <v>8.9468750000000004</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="A143">
-            <v>2041</v>
-          </cell>
-          <cell r="B143">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C143">
-            <v>12.25</v>
-          </cell>
-          <cell r="D143">
-            <v>8.3171874999999993</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="A144">
-            <v>2042</v>
-          </cell>
-          <cell r="B144">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C144">
-            <v>12</v>
-          </cell>
-          <cell r="D144">
-            <v>7.6875</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="A145">
-            <v>2043</v>
-          </cell>
-          <cell r="B145">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C145">
-            <v>11.75</v>
-          </cell>
-          <cell r="D145">
-            <v>7.0578124999999998</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="A146">
-            <v>2044</v>
-          </cell>
-          <cell r="B146">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C146">
-            <v>11.5</v>
-          </cell>
-          <cell r="D146">
-            <v>6.4281249999999996</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="A147">
-            <v>2045</v>
-          </cell>
-          <cell r="B147">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C147">
-            <v>11.25</v>
-          </cell>
-          <cell r="D147">
-            <v>5.7984374999999995</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="A148">
-            <v>2046</v>
-          </cell>
-          <cell r="B148">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C148">
-            <v>11</v>
-          </cell>
-          <cell r="D148">
-            <v>5.1687499999999993</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="A149">
-            <v>2047</v>
-          </cell>
-          <cell r="B149">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C149">
-            <v>10.75</v>
-          </cell>
-          <cell r="D149">
-            <v>4.5390625</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="A150">
-            <v>2048</v>
-          </cell>
-          <cell r="B150">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C150">
-            <v>10.5</v>
-          </cell>
-          <cell r="D150">
-            <v>3.9093749999999998</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="A151">
-            <v>2049</v>
-          </cell>
-          <cell r="B151">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C151">
-            <v>10.25</v>
-          </cell>
-          <cell r="D151">
-            <v>3.2796874999999996</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="A152">
-            <v>2050</v>
-          </cell>
-          <cell r="B152">
-            <v>16.812549695425925</v>
-          </cell>
-          <cell r="C152">
-            <v>10</v>
-          </cell>
-          <cell r="D152">
-            <v>2.65</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7736,15 +7001,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B104145-72CF-4536-9B2E-C849D28231C3}">
   <dimension ref="A1:D152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>63</v>
@@ -9266,7 +8531,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>1989</v>
       </c>
@@ -9283,7 +8548,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>1990</v>
       </c>
@@ -9300,7 +8565,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>1991</v>
       </c>
@@ -9317,7 +8582,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>1992</v>
       </c>
@@ -9334,7 +8599,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>1993</v>
       </c>
@@ -9351,7 +8616,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>1994</v>
       </c>
@@ -9368,7 +8633,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>1995</v>
       </c>
@@ -9385,7 +8650,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>1996</v>
       </c>
@@ -9402,7 +8667,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>1997</v>
       </c>
@@ -9419,7 +8684,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>1998</v>
       </c>
@@ -9436,7 +8701,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>1999</v>
       </c>
@@ -9453,7 +8718,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>2000</v>
       </c>
@@ -9470,7 +8735,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2001</v>
       </c>
@@ -9487,7 +8752,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2002</v>
       </c>
@@ -9504,7 +8769,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2003</v>
       </c>
@@ -9521,7 +8786,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>2004</v>
       </c>
@@ -9538,7 +8803,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2005</v>
       </c>
@@ -9555,7 +8820,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2006</v>
       </c>
@@ -9572,7 +8837,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2007</v>
       </c>
@@ -9589,7 +8854,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>2008</v>
       </c>
@@ -9606,7 +8871,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2009</v>
       </c>
@@ -9623,7 +8888,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2010</v>
       </c>
@@ -9640,7 +8905,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>2011</v>
       </c>
@@ -9657,7 +8922,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>2012</v>
       </c>
@@ -9674,7 +8939,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>2013</v>
       </c>
@@ -9691,7 +8956,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>2014</v>
       </c>
@@ -9708,7 +8973,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>2015</v>
       </c>
@@ -9725,7 +8990,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>2016</v>
       </c>
@@ -9742,7 +9007,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>2017</v>
       </c>
@@ -9759,7 +9024,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>2018</v>
       </c>
@@ -9776,7 +9041,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>2019</v>
       </c>
@@ -9793,7 +9058,7 @@
         <v>0.88593749999999993</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>2020</v>
       </c>
@@ -9810,7 +9075,7 @@
         <v>0.87187499999999996</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2021</v>
       </c>
@@ -9827,7 +9092,7 @@
         <v>0.85781249999999987</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>2022</v>
       </c>
@@ -9844,7 +9109,7 @@
         <v>0.84374999999999978</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>2023</v>
       </c>
@@ -9861,7 +9126,7 @@
         <v>0.8296874999999998</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>2024</v>
       </c>
@@ -9878,7 +9143,7 @@
         <v>0.81562499999999982</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>2025</v>
       </c>
@@ -9895,7 +9160,7 @@
         <v>0.80156249999999973</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>2026</v>
       </c>
@@ -9912,7 +9177,7 @@
         <v>0.78749999999999964</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>2027</v>
       </c>
@@ -9929,7 +9194,7 @@
         <v>0.77343749999999967</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>2028</v>
       </c>
@@ -9946,7 +9211,7 @@
         <v>0.75937499999999969</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2029</v>
       </c>
@@ -9963,7 +9228,7 @@
         <v>0.7453124999999996</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2030</v>
       </c>
@@ -9980,7 +9245,7 @@
         <v>0.73124999999999951</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>2031</v>
       </c>
@@ -9997,7 +9262,7 @@
         <v>0.71718749999999953</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>2032</v>
       </c>
@@ -10014,7 +9279,7 @@
         <v>0.70312499999999956</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>2033</v>
       </c>
@@ -10031,7 +9296,7 @@
         <v>0.68906249999999947</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>2034</v>
       </c>
@@ -10048,7 +9313,7 @@
         <v>0.67499999999999938</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>2035</v>
       </c>
@@ -10065,7 +9330,7 @@
         <v>0.6609374999999994</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>2036</v>
       </c>
@@ -10082,7 +9347,7 @@
         <v>0.64687499999999942</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2037</v>
       </c>
@@ -10099,7 +9364,7 @@
         <v>0.63281249999999933</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>2038</v>
       </c>
@@ -10116,7 +9381,7 @@
         <v>0.61874999999999925</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>2039</v>
       </c>
@@ -10133,7 +9398,7 @@
         <v>0.60468749999999927</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>2040</v>
       </c>
@@ -10150,7 +9415,7 @@
         <v>0.59062499999999929</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>2041</v>
       </c>
@@ -10167,7 +9432,7 @@
         <v>0.5765624999999992</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>2042</v>
       </c>
@@ -10184,7 +9449,7 @@
         <v>0.56249999999999911</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>2043</v>
       </c>
@@ -10201,7 +9466,7 @@
         <v>0.54843749999999913</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>2044</v>
       </c>
@@ -10218,7 +9483,7 @@
         <v>0.53437499999999916</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2045</v>
       </c>
@@ -10235,7 +9500,7 @@
         <v>0.52031249999999907</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>2046</v>
       </c>
@@ -10252,7 +9517,7 @@
         <v>0.50624999999999898</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2047</v>
       </c>
@@ -10269,7 +9534,7 @@
         <v>0.492187499999999</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>2048</v>
       </c>
@@ -10286,7 +9551,7 @@
         <v>0.47812499999999897</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>2049</v>
       </c>
@@ -10303,7 +9568,7 @@
         <v>0.46406249999999893</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>2050</v>
       </c>

</xml_diff>